<commit_message>
modify SessionManager temp Clear
</commit_message>
<xml_diff>
--- a/Protocol.xlsx
+++ b/Protocol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\yuhan\GITHUB\YuhanLH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3679756D-173A-45C2-BE97-0DF5384786AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAA97B6-A9DF-4C54-A15F-863131C2E715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F63FB4D-88F6-4272-BA62-1CE882951EA8}"/>
+    <workbookView xWindow="-26955" yWindow="2085" windowWidth="24600" windowHeight="13800" xr2:uid="{7F63FB4D-88F6-4272-BA62-1CE882951EA8}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol (2)" sheetId="3" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="149">
   <si>
     <t/>
   </si>
@@ -637,10 +637,6 @@
   </si>
   <si>
     <t>SS_LoginFailed</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>t</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
@@ -781,7 +777,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -808,6 +804,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -972,7 +974,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1083,6 +1085,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1630,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD18F077-74E5-4E23-B0EE-B8DD7D2BBFBA}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1650,8 +1655,8 @@
     <col min="10" max="10" width="67.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:14" ht="39" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="34" t="s">
         <v>137</v>
       </c>
@@ -1664,7 +1669,7 @@
       <c r="I2" s="35"/>
       <c r="J2" s="36"/>
     </row>
-    <row r="3" spans="2:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -1675,7 +1680,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>128</v>
       </c>
@@ -1694,7 +1699,7 @@
       </c>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>130</v>
       </c>
@@ -1709,11 +1714,8 @@
         <v>90</v>
       </c>
       <c r="H5" s="10"/>
-      <c r="N5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>132</v>
       </c>
@@ -1727,7 +1729,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>133</v>
       </c>
@@ -1736,12 +1738,12 @@
       </c>
       <c r="E7" s="27"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B9" s="14" t="s">
         <v>1</v>
       </c>
@@ -1754,7 +1756,7 @@
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>20</v>
       </c>
@@ -1783,7 +1785,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="37"/>
       <c r="B11" s="8" t="s">
         <v>2</v>
       </c>
@@ -1808,7 +1811,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="37"/>
       <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
@@ -1829,7 +1833,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="37"/>
       <c r="B13" s="8" t="s">
         <v>16</v>
       </c>
@@ -1858,7 +1863,8 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="37"/>
       <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
@@ -1887,7 +1893,8 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="37"/>
       <c r="B15" s="8" t="s">
         <v>18</v>
       </c>
@@ -1912,7 +1919,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="37"/>
       <c r="B16" s="8" t="s">
         <v>40</v>
       </c>
@@ -1929,7 +1937,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="37"/>
       <c r="B17" s="8" t="s">
         <v>19</v>
       </c>
@@ -1946,12 +1955,13 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="37"/>
       <c r="B18" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>147</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>148</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -1961,7 +1971,7 @@
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
@@ -1972,7 +1982,7 @@
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
     </row>
-    <row r="20" spans="2:10" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
         <v>3</v>
       </c>
@@ -1987,7 +1997,7 @@
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
         <v>20</v>
       </c>
@@ -2014,7 +2024,8 @@
       </c>
       <c r="J21" s="15"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="37"/>
       <c r="B22" s="8" t="s">
         <v>98</v>
       </c>
@@ -2035,7 +2046,8 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="37"/>
       <c r="B23" s="8" t="s">
         <v>97</v>
       </c>
@@ -2060,7 +2072,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="37"/>
       <c r="B24" s="8" t="s">
         <v>5</v>
       </c>
@@ -2080,10 +2093,11 @@
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="37"/>
       <c r="B25" s="8" t="s">
         <v>6</v>
       </c>
@@ -2108,7 +2122,8 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="37"/>
       <c r="B26" s="8" t="s">
         <v>85</v>
       </c>
@@ -2129,7 +2144,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="37"/>
       <c r="B27" s="8" t="s">
         <v>86</v>
       </c>
@@ -2150,7 +2166,8 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="37"/>
       <c r="B28" s="8" t="s">
         <v>87</v>
       </c>
@@ -2175,7 +2192,8 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="37"/>
       <c r="B29" s="8" t="s">
         <v>88</v>
       </c>
@@ -2200,7 +2218,8 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="37"/>
       <c r="B30" s="8" t="s">
         <v>89</v>
       </c>
@@ -2229,7 +2248,8 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="37"/>
       <c r="B31" s="19" t="s">
         <v>64</v>
       </c>
@@ -2250,7 +2270,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B32" s="19" t="s">
         <v>108</v>
       </c>
@@ -2348,6 +2368,7 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="37"/>
       <c r="B36" s="8" t="s">
         <v>4</v>
       </c>
@@ -2373,6 +2394,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="37"/>
       <c r="B37" s="8" t="s">
         <v>45</v>
       </c>
@@ -2396,6 +2418,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="37"/>
       <c r="B38" s="8" t="s">
         <v>115</v>
       </c>
@@ -2419,6 +2442,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="37"/>
       <c r="B39" s="8" t="s">
         <v>8</v>
       </c>
@@ -2442,6 +2466,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="37"/>
       <c r="B40" s="8" t="s">
         <v>76</v>
       </c>
@@ -2467,6 +2492,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="37"/>
       <c r="B41" s="8" t="s">
         <v>77</v>
       </c>
@@ -2488,6 +2514,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="37"/>
       <c r="B42" s="8" t="s">
         <v>78</v>
       </c>
@@ -2597,6 +2624,7 @@
       <c r="J46" s="15"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="37"/>
       <c r="B47" s="8" t="s">
         <v>127</v>
       </c>
@@ -2618,6 +2646,7 @@
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="37"/>
       <c r="B48" s="8" t="s">
         <v>4</v>
       </c>
@@ -2638,7 +2667,8 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" s="37"/>
       <c r="B49" s="12" t="s">
         <v>69</v>
       </c>
@@ -2663,7 +2693,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="2:10" ht="27" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="27" x14ac:dyDescent="0.3">
       <c r="B50" s="12" t="s">
         <v>11</v>
       </c>
@@ -2688,7 +2718,8 @@
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A51" s="37"/>
       <c r="B51" s="13" t="s">
         <v>16</v>
       </c>
@@ -2713,7 +2744,8 @@
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A52" s="37"/>
       <c r="B52" s="13" t="s">
         <v>17</v>
       </c>
@@ -2738,12 +2770,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A53" s="37"/>
       <c r="B53" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="8"/>
@@ -2753,7 +2786,7 @@
       <c r="I53" s="8"/>
       <c r="J53" s="8"/>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
     </row>

</xml_diff>